<commit_message>
updating sweep elimination lists
</commit_message>
<xml_diff>
--- a/Other_workbooks/fiberVolleyCellList.xlsx
+++ b/Other_workbooks/fiberVolleyCellList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="127">
   <si>
     <t>Mouse Name</t>
   </si>
@@ -331,12 +331,87 @@
   <si>
     <t>2015_01_08_0010</t>
   </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>7,9,11,12,13,15,16,17</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>31,42,101</t>
+  </si>
+  <si>
+    <t>54,118</t>
+  </si>
+  <si>
+    <t>41,75,137</t>
+  </si>
+  <si>
+    <t>88,89,90,125</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>23,26,29,</t>
+  </si>
+  <si>
+    <t>1,28,</t>
+  </si>
+  <si>
+    <t>16,27,28,32,74</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>53,92</t>
+  </si>
+  <si>
+    <t>47,118</t>
+  </si>
+  <si>
+    <t>16,75</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>11,13</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>1:20,24</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -362,6 +437,11 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -427,7 +507,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -508,6 +588,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -857,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -870,7 +959,7 @@
     <col min="5" max="5" width="19.28515625" style="26" customWidth="1"/>
     <col min="6" max="7" width="8.85546875" style="27"/>
     <col min="8" max="8" width="8.85546875" style="25"/>
-    <col min="9" max="9" width="12" style="25" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="25" customWidth="1"/>
     <col min="10" max="10" width="38.7109375" style="26" customWidth="1"/>
     <col min="11" max="1025" width="8.85546875" style="28"/>
     <col min="1026" max="16384" width="8.85546875" style="29"/>
@@ -25981,7 +26070,9 @@
       <c r="H26" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="12"/>
+      <c r="I26" s="31" t="s">
+        <v>123</v>
+      </c>
       <c r="J26" s="14"/>
       <c r="K26" s="16"/>
       <c r="L26" s="16"/>
@@ -27024,7 +27115,9 @@
       <c r="H27" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="12"/>
+      <c r="I27" s="31" t="s">
+        <v>124</v>
+      </c>
       <c r="J27" s="14"/>
       <c r="K27" s="16"/>
       <c r="L27" s="16"/>
@@ -29110,8 +29203,8 @@
       <c r="H29" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I29" s="18" t="s">
-        <v>45</v>
+      <c r="I29" s="32" t="s">
+        <v>125</v>
       </c>
       <c r="J29" s="20"/>
       <c r="K29" s="22"/>
@@ -30155,7 +30248,9 @@
       <c r="H30" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I30" s="18"/>
+      <c r="I30" s="32" t="s">
+        <v>126</v>
+      </c>
       <c r="J30" s="20"/>
       <c r="K30" s="22"/>
       <c r="L30" s="22"/>
@@ -33284,7 +33379,9 @@
       <c r="H33" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="6"/>
+      <c r="I33" s="30" t="s">
+        <v>122</v>
+      </c>
       <c r="J33" s="8"/>
       <c r="K33" s="10"/>
       <c r="L33" s="10"/>
@@ -38481,7 +38578,7 @@
       <c r="B38" s="13">
         <v>1</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="31" t="s">
         <v>62</v>
       </c>
       <c r="D38" s="12" t="s">
@@ -38499,7 +38596,9 @@
       <c r="H38" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I38" s="12"/>
+      <c r="I38" s="31" t="s">
+        <v>118</v>
+      </c>
       <c r="J38" s="14"/>
       <c r="K38" s="16"/>
       <c r="L38" s="16"/>
@@ -39542,7 +39641,9 @@
       <c r="H39" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I39" s="12"/>
+      <c r="I39" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="J39" s="14"/>
       <c r="K39" s="16"/>
       <c r="L39" s="16"/>
@@ -40585,7 +40686,9 @@
       <c r="H40" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="12"/>
+      <c r="I40" s="31" t="s">
+        <v>120</v>
+      </c>
       <c r="J40" s="14"/>
       <c r="K40" s="16"/>
       <c r="L40" s="16"/>
@@ -41628,7 +41731,9 @@
       <c r="H41" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I41" s="12"/>
+      <c r="I41" s="31" t="s">
+        <v>121</v>
+      </c>
       <c r="J41" s="14"/>
       <c r="K41" s="16"/>
       <c r="L41" s="16"/>
@@ -42671,7 +42776,9 @@
       <c r="H42" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="I42" s="18"/>
+      <c r="I42" s="32" t="s">
+        <v>115</v>
+      </c>
       <c r="J42" s="20"/>
       <c r="K42" s="22"/>
       <c r="L42" s="22"/>
@@ -44739,7 +44846,7 @@
       <c r="B44" s="21">
         <v>3</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="C44" s="32" t="s">
         <v>70</v>
       </c>
       <c r="D44" s="18" t="s">
@@ -44757,7 +44864,9 @@
       <c r="H44" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="I44" s="18"/>
+      <c r="I44" s="32" t="s">
+        <v>116</v>
+      </c>
       <c r="J44" s="20"/>
       <c r="K44" s="22"/>
       <c r="L44" s="22"/>
@@ -45800,7 +45909,9 @@
       <c r="H45" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="I45" s="18"/>
+      <c r="I45" s="32" t="s">
+        <v>117</v>
+      </c>
       <c r="J45" s="20"/>
       <c r="K45" s="22"/>
       <c r="L45" s="22"/>
@@ -49972,7 +50083,9 @@
       <c r="H49" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I49" s="6"/>
+      <c r="I49" s="30" t="s">
+        <v>114</v>
+      </c>
       <c r="J49" s="8"/>
       <c r="K49" s="10"/>
       <c r="L49" s="10"/>
@@ -52058,7 +52171,9 @@
       <c r="H51" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I51" s="6"/>
+      <c r="I51" s="30" t="s">
+        <v>112</v>
+      </c>
       <c r="J51" s="8"/>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
@@ -53101,7 +53216,9 @@
       <c r="H52" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I52" s="6"/>
+      <c r="I52" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="J52" s="8"/>
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
@@ -55187,7 +55304,9 @@
       <c r="H54" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="I54" s="12"/>
+      <c r="I54" s="31" t="s">
+        <v>107</v>
+      </c>
       <c r="J54" s="14"/>
       <c r="K54" s="16"/>
       <c r="L54" s="16"/>
@@ -56230,7 +56349,9 @@
       <c r="H55" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="I55" s="12"/>
+      <c r="I55" s="31" t="s">
+        <v>108</v>
+      </c>
       <c r="J55" s="14"/>
       <c r="K55" s="16"/>
       <c r="L55" s="16"/>
@@ -57273,7 +57394,9 @@
       <c r="H56" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="I56" s="12"/>
+      <c r="I56" s="31" t="s">
+        <v>109</v>
+      </c>
       <c r="J56" s="14"/>
       <c r="K56" s="16"/>
       <c r="L56" s="16"/>
@@ -58298,7 +58421,7 @@
       <c r="B57" s="13">
         <v>1</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C57" s="31" t="s">
         <v>88</v>
       </c>
       <c r="D57" s="12" t="s">
@@ -58316,7 +58439,9 @@
       <c r="H57" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="I57" s="12"/>
+      <c r="I57" s="31" t="s">
+        <v>110</v>
+      </c>
       <c r="J57" s="14"/>
       <c r="K57" s="16"/>
       <c r="L57" s="16"/>
@@ -61445,7 +61570,9 @@
       <c r="H60" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="I60" s="18"/>
+      <c r="I60" s="32" t="s">
+        <v>111</v>
+      </c>
       <c r="J60" s="20"/>
       <c r="K60" s="22"/>
       <c r="L60" s="22"/>
@@ -64574,7 +64701,9 @@
       <c r="H63" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I63" s="6"/>
+      <c r="I63" s="30" t="s">
+        <v>102</v>
+      </c>
       <c r="J63" s="8"/>
       <c r="K63" s="10"/>
       <c r="L63" s="10"/>
@@ -65617,7 +65746,9 @@
       <c r="H64" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I64" s="6"/>
+      <c r="I64" s="30" t="s">
+        <v>103</v>
+      </c>
       <c r="J64" s="8"/>
       <c r="K64" s="10"/>
       <c r="L64" s="10"/>
@@ -67685,7 +67816,7 @@
       <c r="B66" s="13">
         <v>2</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="31" t="s">
         <v>98</v>
       </c>
       <c r="D66" s="12" t="s">
@@ -68746,7 +68877,9 @@
       <c r="H67" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="I67" s="12"/>
+      <c r="I67" s="31" t="s">
+        <v>104</v>
+      </c>
       <c r="J67" s="14"/>
       <c r="K67" s="16"/>
       <c r="L67" s="16"/>
@@ -69789,7 +69922,9 @@
       <c r="H68" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="I68" s="12"/>
+      <c r="I68" s="31" t="s">
+        <v>105</v>
+      </c>
       <c r="J68" s="14"/>
       <c r="K68" s="16"/>
       <c r="L68" s="16"/>
@@ -70832,7 +70967,9 @@
       <c r="H69" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="I69" s="12"/>
+      <c r="I69" s="31" t="s">
+        <v>106</v>
+      </c>
       <c r="J69" s="14"/>
       <c r="K69" s="16"/>
       <c r="L69" s="16"/>
@@ -71852,7 +71989,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>